<commit_message>
Data 1 and 2
</commit_message>
<xml_diff>
--- a/dataset/Correlations/Data 1 Correlations.xlsx
+++ b/dataset/Correlations/Data 1 Correlations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manar 2\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manar 2\Desktop\Winter Semester\CISC 850 - Cyber Physical Security\Project\Shared Files\GitHub\False-Data-Injection-Detection-for-Smart-Grid-Systems\dataset\Correlations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09058657-F67D-46A8-8847-9178DE25841D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BE97CE-8296-44D8-BBF1-62CBB203FDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -451,6 +451,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -761,11 +766,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DU125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:DT125"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="125" max="125" width="16.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:125">
       <c r="A1" s="1" t="s">
@@ -43609,6 +43617,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:DT125">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00FF00"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>